<commit_message>
OCR extraction with document_no validation: min_digits=4, skip_lines=3, improved tax_id patterns
</commit_message>
<xml_diff>
--- a/Vendor_branch.xlsx
+++ b/Vendor_branch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ocr\view_ocr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA5437B-C5DC-4F76-BC18-A4F602D85F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA7ED43-C2D7-4DA8-9175-8EC148CC1FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6506BE60-3C73-4701-8988-81E5CDE8235E}"/>
+    <workbookView xWindow="915" yWindow="1740" windowWidth="14310" windowHeight="11295" xr2:uid="{6506BE60-3C73-4701-8988-81E5CDE8235E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="154">
   <si>
     <t>เลขประจำตัวผู้เสียภาษี</t>
   </si>
@@ -480,6 +480,24 @@
   </si>
   <si>
     <t>บริษัท ซีพี ออลล์ จำกัด (มหาชน)</t>
+  </si>
+  <si>
+    <t>0125545006558</t>
+  </si>
+  <si>
+    <t>บริษัท ปังปอน จำกัด</t>
+  </si>
+  <si>
+    <t>PON001</t>
+  </si>
+  <si>
+    <t>0115564018396</t>
+  </si>
+  <si>
+    <t>บริษัท ซิณี เพรสทิจ จำกัด</t>
+  </si>
+  <si>
+    <t>PS001</t>
   </si>
 </sst>
 </file>
@@ -564,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -602,6 +620,7 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -669,6 +688,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -740,8 +760,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AD0FC8F-5EBA-45F3-BFB6-3B5777E0DD0A}" name="Table13" displayName="Table13" ref="A1:E49" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:E49" xr:uid="{4AD0FC8F-5EBA-45F3-BFB6-3B5777E0DD0A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AD0FC8F-5EBA-45F3-BFB6-3B5777E0DD0A}" name="Table13" displayName="Table13" ref="A1:E51" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:E51" xr:uid="{4AD0FC8F-5EBA-45F3-BFB6-3B5777E0DD0A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A9401744-4D9B-481D-AC6A-B9499EB63AFF}" name="เลขประจำตัวผู้เสียภาษี" dataDxfId="4" dataCellStyle="Comma"/>
     <tableColumn id="2" xr3:uid="{E9821A21-10F9-47B5-9D0A-D7306A5FC04F}" name="ชื่อบริษัท" dataDxfId="3"/>
@@ -1070,17 +1090,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11ACC454-015B-4582-9B54-6E306FF53C87}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.625" customWidth="1"/>
+    <col min="1" max="1" width="21.625" style="15" customWidth="1"/>
     <col min="2" max="2" width="38.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.75" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.75" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
   </cols>
@@ -1916,6 +1936,40 @@
       </c>
       <c r="E49" s="14" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OCR logic: Simplify Doc Types, Refine Extraction, Custom Excel Output
- Simplify Document Types to Invoice, CY Instruction, Billing Note

- Update Excel output to 3 separate sheets with custom columns

- Refine CY Booking extraction (regex + space removal)

- Refine Billing Note extraction (skip header lines)

- Update UI Settings in app.py
</commit_message>
<xml_diff>
--- a/Vendor_branch.xlsx
+++ b/Vendor_branch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ocr\view_ocr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ocr\ocr_cpi_exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA7ED43-C2D7-4DA8-9175-8EC148CC1FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1C5C0D-12C0-4115-A727-F7FE22CE33DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="1740" windowWidth="14310" windowHeight="11295" xr2:uid="{6506BE60-3C73-4701-8988-81E5CDE8235E}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="31196" windowHeight="16917" xr2:uid="{6506BE60-3C73-4701-8988-81E5CDE8235E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,13 +506,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="00000"/>
+    <numFmt numFmtId="187" formatCode="00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -520,7 +520,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -541,7 +541,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -549,7 +549,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -606,7 +606,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -662,7 +662,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="00000"/>
+      <numFmt numFmtId="187" formatCode="00000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1092,20 +1092,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11ACC454-015B-4582-9B54-6E306FF53C87}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="38.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="38.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.69921875" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>83</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>84</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>85</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>86</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>87</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>88</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>50</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>51</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>52</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>52</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>53</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>55</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>56</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>57</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>60</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>61</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>62</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>63</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>64</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>65</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>66</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>67</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>68</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>69</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
         <v>70</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
         <v>72</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
         <v>73</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>74</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="s">
         <v>75</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
         <v>76</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>5</v>
@@ -1785,7 +1785,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
         <v>77</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
         <v>78</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>78</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="s">
         <v>79</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A45" s="4" t="s">
         <v>80</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A46" s="4" t="s">
         <v>81</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>82</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>95</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
         <v>145</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
         <v>148</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="16.95" x14ac:dyDescent="0.4">
       <c r="A51" s="4" t="s">
         <v>151</v>
       </c>
@@ -1981,6 +1981,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="9ea82972-d7d5-4eaf-919e-93bb6e68076d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cd7e064-e400-4284-9400-fb553c28cffa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000415EE01BF4D804280F380F9DB1CFF0D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a0889e59f2beebff0116b3924e2bba8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0cd7e064-e400-4284-9400-fb553c28cffa" xmlns:ns3="9ea82972-d7d5-4eaf-919e-93bb6e68076d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a759d0038229a5f52eef73949470c7e5" ns2:_="" ns3:_="">
     <xsd:import namespace="0cd7e064-e400-4284-9400-fb553c28cffa"/>
@@ -2175,27 +2195,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="9ea82972-d7d5-4eaf-919e-93bb6e68076d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cd7e064-e400-4284-9400-fb553c28cffa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1C2E36A-EC7F-423F-8D14-19D21DB059CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5149320-348A-41FF-9075-6A0A41134A26}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9ea82972-d7d5-4eaf-919e-93bb6e68076d"/>
+    <ds:schemaRef ds:uri="0cd7e064-e400-4284-9400-fb553c28cffa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25A85255-B37F-41AE-9392-794E41C222F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2212,23 +2231,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5149320-348A-41FF-9075-6A0A41134A26}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9ea82972-d7d5-4eaf-919e-93bb6e68076d"/>
-    <ds:schemaRef ds:uri="0cd7e064-e400-4284-9400-fb553c28cffa"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1C2E36A-EC7F-423F-8D14-19D21DB059CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>